<commit_message>
updated AVCDL vendor CMM template spreadsheet (error in column header)
</commit_message>
<xml_diff>
--- a/distribution/reference_documents/templates/AVCDL vendor CMM template.xlsx
+++ b/distribution/reference_documents/templates/AVCDL vendor CMM template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charleswilson/Documents/projects/AVCDL/distribution/reference_documents/cybersecurity_interface_agreement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles.wilson/Documents/projects/AVCDL/source/reference_documents/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FB2816-A59D-E642-8D7D-2277F687DEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5E631F-30C2-A349-BD0C-481F07F312D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9520" yWindow="2680" windowWidth="38760" windowHeight="27000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,9 +46,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Work Product</t>
-  </si>
-  <si>
     <t>CMM Level</t>
   </si>
   <si>
@@ -472,7 +469,10 @@
     <t>list of tools and components used</t>
   </si>
   <si>
-    <t>revision 3</t>
+    <t>AVCDL Product</t>
+  </si>
+  <si>
+    <t>revision 4</t>
   </si>
 </sst>
 </file>
@@ -704,6 +704,43 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -728,45 +765,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
@@ -1010,810 +1010,810 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="F1" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="B3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="18"/>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="C7" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="18"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="18"/>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="18"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="18"/>
+      <c r="B22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="18"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="18"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="18"/>
+      <c r="B27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="31"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="33"/>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="4" t="s">
+      <c r="E29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="18"/>
+      <c r="B30" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="18"/>
+      <c r="B31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="18"/>
+      <c r="B32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="18"/>
+      <c r="B33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
-      <c r="B13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
-      <c r="B14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
-      <c r="B19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="E33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="18"/>
+      <c r="B34" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="18"/>
+      <c r="B35" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="18"/>
+      <c r="B36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="18"/>
+      <c r="B37" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="18"/>
+      <c r="B38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="18"/>
+      <c r="B39" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
-      <c r="B22" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
-      <c r="B24" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
-      <c r="B27" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="20"/>
-    </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="22"/>
-      <c r="B30" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="11"/>
-    </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="22"/>
-      <c r="B31" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="11"/>
-    </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="22"/>
-      <c r="B32" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="22"/>
-      <c r="B33" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="11"/>
-    </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="22"/>
-      <c r="B34" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="11"/>
-    </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="22"/>
-      <c r="B35" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="11"/>
-    </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="22"/>
-      <c r="B36" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="11"/>
-    </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="22"/>
-      <c r="B37" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="11"/>
-    </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="22"/>
-      <c r="B38" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="E39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="31"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="33"/>
+    </row>
+    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="11"/>
+    </row>
+    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="17"/>
+      <c r="B42" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="11"/>
-    </row>
-    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="22"/>
-      <c r="B39" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="11"/>
-    </row>
-    <row r="40" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="20"/>
-    </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="C42" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="11"/>
+    </row>
+    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="17"/>
+      <c r="B43" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E41" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="11"/>
-    </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
-      <c r="B42" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D42" s="4" t="s">
+      <c r="C43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="11"/>
+    </row>
+    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="17"/>
+      <c r="B44" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="11"/>
-    </row>
-    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="21"/>
-      <c r="B43" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="11"/>
-    </row>
-    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
-      <c r="B44" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="7" t="s">
+      <c r="D44" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="11"/>
+    </row>
+    <row r="45" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="31"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
+    </row>
+    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="11"/>
-    </row>
-    <row r="45" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="20"/>
-    </row>
-    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
+      <c r="B46" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="E46" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="11"/>
+    </row>
+    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="18"/>
+      <c r="B47" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="11"/>
-    </row>
-    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="22"/>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="E47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="11"/>
+    </row>
+    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="18"/>
+      <c r="B48" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E47" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="11"/>
-    </row>
-    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="22"/>
-      <c r="B48" s="9" t="s">
+      <c r="C48" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="D48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="11"/>
+    </row>
+    <row r="49" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="31"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
+    </row>
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="11"/>
-    </row>
-    <row r="49" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="20"/>
-    </row>
-    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="21" t="s">
+      <c r="B50" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="C50" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D50" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="D50" s="23" t="s">
+      <c r="E50" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="26"/>
+    </row>
+    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="18"/>
+      <c r="B51" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="13"/>
-    </row>
-    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="22"/>
-      <c r="B51" s="6" t="s">
+      <c r="C51" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="D51" s="18"/>
+      <c r="E51" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="27"/>
+    </row>
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="18"/>
+      <c r="B52" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D51" s="22"/>
-      <c r="E51" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="14"/>
-    </row>
-    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="22"/>
-      <c r="B52" s="6" t="s">
+      <c r="C52" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="D52" s="18"/>
+      <c r="E52" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="27"/>
+    </row>
+    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="18"/>
+      <c r="B53" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D52" s="22"/>
-      <c r="E52" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="14"/>
-    </row>
-    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="22"/>
-      <c r="B53" s="6" t="s">
+      <c r="C53" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="E53" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="28"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="30"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="15"/>
     </row>
     <row r="55" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="C55" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="D55" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="E55" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" s="11"/>
     </row>
@@ -5574,6 +5574,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="A54:F54"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A3:A15"/>
@@ -5590,22 +5606,6 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="A46:A48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -5643,58 +5643,58 @@
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="36"/>
       <c r="B3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="36"/>
       <c r="B4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="36"/>
       <c r="B5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="36"/>
       <c r="B6" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="36"/>
       <c r="B7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>